<commit_message>
renamed the java page files and tested the add account script
</commit_message>
<xml_diff>
--- a/PFSTestData.xlsx
+++ b/PFSTestData.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\CARE_Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\PFS_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="ActiveData_SingleUser" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,62 +24,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
-  <si>
-    <t>User Name</t>
-  </si>
-  <si>
-    <t>Type of Credentials</t>
-  </si>
-  <si>
-    <t>QA Env</t>
-  </si>
-  <si>
-    <t>Dev Env</t>
-  </si>
-  <si>
-    <t>https://cft-care-dev.g1.app.cloud.comcast.net/login</t>
-  </si>
-  <si>
-    <t>Browser</t>
-  </si>
-  <si>
-    <t>Chrome</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Application URL</t>
   </si>
   <si>
-    <t>Application URLs</t>
-  </si>
-  <si>
-    <t>https://cft-care-qa.g5.app.cloud.comcast.net/login</t>
-  </si>
-  <si>
     <t>https://uat.royalbank.can-act.com</t>
   </si>
   <si>
     <t>Askida2018</t>
   </si>
   <si>
-    <t>UserName_1</t>
-  </si>
-  <si>
-    <t>Password_1</t>
-  </si>
-  <si>
-    <t>UserName_2</t>
-  </si>
-  <si>
-    <t>Password_2</t>
-  </si>
-  <si>
-    <t>33008643-0106</t>
-  </si>
-  <si>
-    <t>Account Type</t>
-  </si>
-  <si>
     <t>Account Number</t>
   </si>
   <si>
@@ -90,6 +45,21 @@
   </si>
   <si>
     <t>33008208</t>
+  </si>
+  <si>
+    <t>Edit Account Number</t>
+  </si>
+  <si>
+    <t>Pyament Type</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>123481731SL0008</t>
   </si>
 </sst>
 </file>
@@ -133,7 +103,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -156,36 +126,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -470,122 +424,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B14" r:id="rId1"/>
-    <hyperlink ref="B15" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added the data of second payment type
</commit_message>
<xml_diff>
--- a/PFSTestData.xlsx
+++ b/PFSTestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Application URL</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>123481731SL0008</t>
+  </si>
+  <si>
+    <t>PEI - 911 Cost Recovery Fee Return -- PEIRF -- (07PT15-16530)</t>
   </si>
 </sst>
 </file>
@@ -132,7 +135,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
@@ -142,6 +145,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -424,11 +428,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -480,11 +482,32 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>33008208</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3">
+        <v>122546113</v>
+      </c>
+      <c r="F3" s="4">
+        <v>741258802</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
managed the Test Methods
</commit_message>
<xml_diff>
--- a/PFSTestData.xlsx
+++ b/PFSTestData.xlsx
@@ -430,9 +430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -465,8 +463,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
+      <c r="A2" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -478,15 +476,15 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>12</v>
+      <c r="A3" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -498,16 +496,16 @@
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Automate 5 scenarios of PFS
</commit_message>
<xml_diff>
--- a/PFSTestData.xlsx
+++ b/PFSTestData.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="ActiveData_SingleUser" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="33">
   <si>
     <t>Application URL</t>
   </si>
@@ -38,15 +39,6 @@
     <t>Account Number</t>
   </si>
   <si>
-    <t>123481731SL0002</t>
-  </si>
-  <si>
-    <t>Federal - Softwood Lumber Products Export Chrg -- SLPEX</t>
-  </si>
-  <si>
-    <t>33008208</t>
-  </si>
-  <si>
     <t>Edit Account Number</t>
   </si>
   <si>
@@ -59,20 +51,86 @@
     <t>Password</t>
   </si>
   <si>
-    <t>123481731SL0008</t>
-  </si>
-  <si>
-    <t>PEI - 911 Cost Recovery Fee Return -- PEIRF -- (07PT15-16530)</t>
-  </si>
-  <si>
-    <t>741258802</t>
+    <t>Payment Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Pyament Type Space</t>
+  </si>
+  <si>
+    <t>123481731RT1013</t>
+  </si>
+  <si>
+    <t>123481731RT1015</t>
+  </si>
+  <si>
+    <t>Federal - GST/HST  Return and Payment -- GST34 -- (GST34)</t>
+  </si>
+  <si>
+    <t>GST34</t>
+  </si>
+  <si>
+    <t>To be processed</t>
+  </si>
+  <si>
+    <t>2020 Dec 31</t>
+  </si>
+  <si>
+    <t>2019 Dec 01</t>
+  </si>
+  <si>
+    <t>33008206</t>
+  </si>
+  <si>
+    <t>payment_type_search</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>ReportingPeriodFrom</t>
+  </si>
+  <si>
+    <t>ReportingPeriodTo</t>
+  </si>
+  <si>
+    <t>2021 Feb 23</t>
+  </si>
+  <si>
+    <t>1034132638TQ0013</t>
+  </si>
+  <si>
+    <t>1034132638TQ0015</t>
+  </si>
+  <si>
+    <t>QUEBEC COMBINED GST/HST + QST REMITTANCE -- G-QST -- (FPZ-500.IF)</t>
+  </si>
+  <si>
+    <t>G-QST</t>
+  </si>
+  <si>
+    <t>9123654789PN0007</t>
+  </si>
+  <si>
+    <t>9123654789PN0008</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quebec Collection of Support Payments -- RPPAQ -- (PPA-101)</t>
+  </si>
+  <si>
+    <t>RPPAQ</t>
+  </si>
+  <si>
+    <t>Quebec Collection of Support Payments -- RPPAQ -- (PPA-101)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,14 +141,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -109,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -132,24 +182,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -428,88 +507,452 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="H2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="F3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+    </row>
+    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="F4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B1" r:id="rId1" display="https://uat.royalbank.can-act.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>